<commit_message>
Aanpassingen PFAS en negatief zwemadviezen
</commit_message>
<xml_diff>
--- a/data/Zwemwater maatregelen vanaf 2012 v2.xlsx
+++ b/data/Zwemwater maatregelen vanaf 2012 v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\wklrap_2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FE2DF3-03DB-4853-968D-6130C28428DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E1B0FF-E74D-4FFD-8525-756414E0F6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2204" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2204" uniqueCount="98">
   <si>
     <t>Meetpunt</t>
   </si>
@@ -295,13 +295,7 @@
     <t>IE 480n/dl</t>
   </si>
   <si>
-    <t>negatief zwemadvies</t>
-  </si>
-  <si>
     <t>ivm drijflaag cat III</t>
-  </si>
-  <si>
-    <t>waarschuwing</t>
   </si>
   <si>
     <t>Som van Dagen</t>
@@ -15937,8 +15931,8 @@
   <dimension ref="A1:H999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H201" sqref="H201"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C187" sqref="C187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16754,7 +16748,7 @@
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C32" t="s">
@@ -16804,7 +16798,7 @@
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C34" t="s">
@@ -16854,7 +16848,7 @@
       <c r="A36" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C36" t="s">
@@ -16904,7 +16898,7 @@
       <c r="A38" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C38" t="s">
@@ -16929,7 +16923,7 @@
       <c r="A39" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C39" t="s">
@@ -16954,7 +16948,7 @@
       <c r="A40" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C40" t="s">
@@ -17029,7 +17023,7 @@
       <c r="A43" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C43" t="s">
@@ -17054,7 +17048,7 @@
       <c r="A44" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C44" t="s">
@@ -17107,7 +17101,7 @@
       <c r="A46" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C46" t="s">
@@ -17157,7 +17151,7 @@
       <c r="A48" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
@@ -17182,7 +17176,7 @@
       <c r="A49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C49" t="s">
@@ -17238,7 +17232,7 @@
       <c r="A51" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C51" t="s">
@@ -17263,7 +17257,7 @@
       <c r="A52" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C52" t="s">
@@ -17291,7 +17285,7 @@
       <c r="A53" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C53" t="s">
@@ -17344,7 +17338,7 @@
       <c r="A55" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C55" t="s">
@@ -17394,7 +17388,7 @@
       <c r="A57" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C57" t="s">
@@ -17419,7 +17413,7 @@
       <c r="A58" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C58" t="s">
@@ -17469,7 +17463,7 @@
       <c r="A60" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C60" t="s">
@@ -17494,7 +17488,7 @@
       <c r="A61" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C61" t="s">
@@ -17544,7 +17538,7 @@
       <c r="A63" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C63" t="s">
@@ -17597,7 +17591,7 @@
       <c r="A65" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C65" t="s">
@@ -17622,7 +17616,7 @@
       <c r="A66" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C66" t="s">
@@ -17675,7 +17669,7 @@
       <c r="A68" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C68" t="s">
@@ -17703,7 +17697,7 @@
       <c r="A69" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C69" t="s">
@@ -17759,7 +17753,7 @@
       <c r="A71" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C71" t="s">
@@ -17784,7 +17778,7 @@
       <c r="A72" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C72" t="s">
@@ -17862,7 +17856,7 @@
       <c r="A75" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C75" t="s">
@@ -17887,7 +17881,7 @@
       <c r="A76" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C76" t="s">
@@ -17912,7 +17906,7 @@
       <c r="A77" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C77" t="s">
@@ -17987,7 +17981,7 @@
       <c r="A80" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C80" t="s">
@@ -18037,7 +18031,7 @@
       <c r="A82" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C82" t="s">
@@ -18062,7 +18056,7 @@
       <c r="A83" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C83" t="s">
@@ -18087,7 +18081,7 @@
       <c r="A84" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C84" t="s">
@@ -18112,7 +18106,7 @@
       <c r="A85" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C85" t="s">
@@ -18140,7 +18134,7 @@
       <c r="A86" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C86" t="s">
@@ -18479,7 +18473,7 @@
       <c r="A99" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C99" t="s">
@@ -18557,7 +18551,7 @@
       <c r="A102" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C102" t="s">
@@ -18633,7 +18627,7 @@
       <c r="A105" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C105" t="s">
@@ -18658,7 +18652,7 @@
       <c r="A106" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C106" t="s">
@@ -18708,7 +18702,7 @@
       <c r="A108" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C108" t="s">
@@ -18758,7 +18752,7 @@
       <c r="A110" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C110" t="s">
@@ -18884,7 +18878,7 @@
       <c r="A115" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C115" t="s">
@@ -18934,7 +18928,7 @@
       <c r="A117" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C117" t="s">
@@ -18959,7 +18953,7 @@
       <c r="A118" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C118" t="s">
@@ -18984,7 +18978,7 @@
       <c r="A119" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C119" t="s">
@@ -19037,7 +19031,7 @@
       <c r="A121" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C121" t="s">
@@ -19137,7 +19131,7 @@
       <c r="A125" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C125" t="s">
@@ -19221,7 +19215,7 @@
       <c r="A128" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C128" t="s">
@@ -19299,7 +19293,7 @@
       <c r="A131" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C131" t="s">
@@ -19349,7 +19343,7 @@
       <c r="A133" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C133" t="s">
@@ -19374,7 +19368,7 @@
       <c r="A134" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C134" t="s">
@@ -19399,7 +19393,7 @@
       <c r="A135" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C135" t="s">
@@ -19502,7 +19496,7 @@
       <c r="A139" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C139" t="s">
@@ -20715,7 +20709,7 @@
       <c r="A184" t="s">
         <v>51</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B184" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C184" t="s">
@@ -20799,7 +20793,7 @@
       <c r="A187" t="s">
         <v>23</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B187" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C187" t="s">
@@ -20874,7 +20868,7 @@
       <c r="A190" t="s">
         <v>12</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B190" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C190" s="4" t="s">
@@ -20949,8 +20943,8 @@
       <c r="A193" t="s">
         <v>51</v>
       </c>
-      <c r="B193" t="s">
-        <v>72</v>
+      <c r="B193" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C193" t="s">
         <v>10</v>
@@ -20962,7 +20956,7 @@
         <v>45526</v>
       </c>
       <c r="F193" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G193">
         <f t="shared" ca="1" si="6"/>
@@ -20977,8 +20971,8 @@
       <c r="A194" t="s">
         <v>51</v>
       </c>
-      <c r="B194" t="s">
-        <v>74</v>
+      <c r="B194" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C194" t="s">
         <v>10</v>
@@ -21002,8 +20996,8 @@
       <c r="A195" t="s">
         <v>15</v>
       </c>
-      <c r="B195" t="s">
-        <v>74</v>
+      <c r="B195" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C195" t="s">
         <v>10</v>
@@ -21027,8 +21021,8 @@
       <c r="A196" t="s">
         <v>23</v>
       </c>
-      <c r="B196" t="s">
-        <v>74</v>
+      <c r="B196" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C196" t="s">
         <v>10</v>
@@ -21052,8 +21046,8 @@
       <c r="A197" t="s">
         <v>12</v>
       </c>
-      <c r="B197" t="s">
-        <v>74</v>
+      <c r="B197" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C197" t="s">
         <v>10</v>
@@ -21077,8 +21071,8 @@
       <c r="A198" t="s">
         <v>51</v>
       </c>
-      <c r="B198" t="s">
-        <v>72</v>
+      <c r="B198" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C198" t="s">
         <v>10</v>
@@ -21102,8 +21096,8 @@
       <c r="A199" t="s">
         <v>51</v>
       </c>
-      <c r="B199" t="s">
-        <v>74</v>
+      <c r="B199" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C199" t="s">
         <v>10</v>
@@ -29141,7 +29135,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" prompt="Nader onderzoek_x000a_Waarschuwing_x000a_Negatief zwemadvies_x000a_Zwemverbod" sqref="B125 B127:B128 B131 B133:B135 B139" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" prompt="Nader onderzoek_x000a_Waarschuwing_x000a_Negatief zwemadvies_x000a_Zwemverbod" sqref="B127" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$K$24:$K$27</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Blauwalg_x000a_Bacteriën_x000a_Zwemmersjeuk_x000a_Jeukklachten" sqref="C2:C999" xr:uid="{00000000-0002-0000-0000-000001000000}">
@@ -29209,13 +29203,13 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D2" s="1">
         <v>41030</v>
@@ -29228,7 +29222,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>2</v>
@@ -29236,13 +29230,13 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D3" s="1">
         <v>41033</v>
@@ -29261,24 +29255,24 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N3" t="s">
         <v>13</v>
       </c>
       <c r="O3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D4" s="1">
         <v>41050</v>
@@ -29291,7 +29285,7 @@
         <v>16</v>
       </c>
       <c r="K4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L4" t="s">
         <v>9</v>
@@ -29308,13 +29302,13 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D5" s="1">
         <v>41079</v>
@@ -29327,7 +29321,7 @@
         <v>23</v>
       </c>
       <c r="K5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M5">
         <v>9</v>
@@ -29341,13 +29335,13 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D6" s="1">
         <v>41121</v>
@@ -29360,7 +29354,7 @@
         <v>9</v>
       </c>
       <c r="K6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L6" t="s">
         <v>9</v>
@@ -29377,7 +29371,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>9</v>
@@ -29399,7 +29393,7 @@
         <v>5</v>
       </c>
       <c r="K7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L7" t="s">
         <v>16</v>
@@ -29413,7 +29407,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>9</v>
@@ -29435,7 +29429,7 @@
         <v>14</v>
       </c>
       <c r="K8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M8">
         <v>34</v>
@@ -29449,13 +29443,13 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D9" s="1">
         <v>41115</v>
@@ -29468,7 +29462,7 @@
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L9" t="s">
         <v>11</v>
@@ -29482,13 +29476,13 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D10" s="1">
         <v>41116</v>
@@ -29504,7 +29498,7 @@
         <v>5</v>
       </c>
       <c r="K10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L10" t="s">
         <v>9</v>
@@ -29518,13 +29512,13 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D11" s="1">
         <v>41121</v>
@@ -29537,7 +29531,7 @@
         <v>9</v>
       </c>
       <c r="K11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M11">
         <v>59</v>
@@ -29548,13 +29542,13 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D12" s="1">
         <v>41131</v>
@@ -29570,7 +29564,7 @@
         <v>17</v>
       </c>
       <c r="K12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L12" t="s">
         <v>11</v>
@@ -29584,13 +29578,13 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D13" s="1">
         <v>41148</v>
@@ -29603,7 +29597,7 @@
         <v>2</v>
       </c>
       <c r="K13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L13" t="s">
         <v>9</v>
@@ -29617,7 +29611,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>9</v>
@@ -29638,7 +29632,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M14">
         <v>57</v>
@@ -29649,13 +29643,13 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D15" s="1">
         <v>41030</v>
@@ -29670,7 +29664,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L15" t="s">
         <v>11</v>
@@ -29684,13 +29678,13 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D16" s="1">
         <v>41033</v>
@@ -29705,7 +29699,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L16" t="s">
         <v>9</v>
@@ -29719,13 +29713,13 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D17" s="8">
         <v>41052</v>
@@ -29741,7 +29735,7 @@
         <v>8</v>
       </c>
       <c r="K17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M17">
         <v>59</v>
@@ -29752,13 +29746,13 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D18" s="1">
         <v>41060</v>
@@ -29771,7 +29765,7 @@
         <v>6</v>
       </c>
       <c r="K18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L18" t="s">
         <v>11</v>
@@ -29785,13 +29779,13 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D19" s="1">
         <v>41079</v>
@@ -29804,7 +29798,7 @@
         <v>23</v>
       </c>
       <c r="K19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L19" t="s">
         <v>9</v>
@@ -29818,13 +29812,13 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D20" s="1">
         <v>41030</v>
@@ -29837,7 +29831,7 @@
         <v>3</v>
       </c>
       <c r="K20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N20">
         <v>19</v>
@@ -29848,13 +29842,13 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D21" s="1">
         <v>41033</v>
@@ -29867,7 +29861,7 @@
         <v>17</v>
       </c>
       <c r="K21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L21" t="s">
         <v>11</v>
@@ -29881,13 +29875,13 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D22" s="1">
         <v>41050</v>
@@ -29900,7 +29894,7 @@
         <v>2</v>
       </c>
       <c r="K22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L22" t="s">
         <v>9</v>
@@ -29914,13 +29908,13 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D23" s="1">
         <v>41052</v>
@@ -29933,7 +29927,7 @@
         <v>8</v>
       </c>
       <c r="K23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M23">
         <v>115</v>
@@ -29944,13 +29938,13 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D24" s="1">
         <v>41060</v>
@@ -29965,13 +29959,13 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D25" s="1">
         <v>41079</v>
@@ -29986,7 +29980,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>9</v>
@@ -30010,7 +30004,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>11</v>
@@ -30034,13 +30028,13 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D28" s="1">
         <v>41052</v>
@@ -30055,13 +30049,13 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D29" s="1">
         <v>41079</v>
@@ -30076,13 +30070,13 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D30" s="1">
         <v>41148</v>
@@ -30097,13 +30091,13 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D31" s="1">
         <v>41150</v>
@@ -30159,12 +30153,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -30172,7 +30166,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -30180,7 +30174,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -30188,7 +30182,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -30196,7 +30190,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -30204,7 +30198,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -30212,7 +30206,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
@@ -30220,7 +30214,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
@@ -30228,7 +30222,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
@@ -33359,7 +33353,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -33372,7 +33366,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>1</v>
@@ -33430,7 +33424,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
@@ -33563,7 +33557,7 @@
     </row>
     <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
@@ -33586,7 +33580,7 @@
     </row>
     <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
@@ -33609,7 +33603,7 @@
     </row>
     <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>9</v>
@@ -33632,7 +33626,7 @@
     </row>
     <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>9</v>
@@ -33655,7 +33649,7 @@
     </row>
     <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>9</v>
@@ -33678,7 +33672,7 @@
     </row>
     <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>9</v>
@@ -33704,7 +33698,7 @@
     </row>
     <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>9</v>
@@ -33730,7 +33724,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>9</v>
@@ -33753,7 +33747,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>16</v>
@@ -33779,7 +33773,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>9</v>
@@ -33802,7 +33796,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>16</v>
@@ -33828,7 +33822,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>9</v>
@@ -33851,7 +33845,7 @@
     </row>
     <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>9</v>
@@ -33874,7 +33868,7 @@
     </row>
     <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>9</v>
@@ -33897,7 +33891,7 @@
     </row>
     <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>11</v>
@@ -33920,7 +33914,7 @@
     </row>
     <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>11</v>
@@ -33946,7 +33940,7 @@
     </row>
     <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>9</v>
@@ -33969,7 +33963,7 @@
     </row>
     <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>9</v>
@@ -33992,7 +33986,7 @@
     </row>
     <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>9</v>
@@ -34015,7 +34009,7 @@
     </row>
     <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>11</v>
@@ -34038,7 +34032,7 @@
     </row>
     <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>9</v>
@@ -34061,7 +34055,7 @@
     </row>
     <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>11</v>
@@ -34084,7 +34078,7 @@
     </row>
     <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>9</v>
@@ -34107,7 +34101,7 @@
     </row>
     <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>9</v>
@@ -34130,7 +34124,7 @@
     </row>
     <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>9</v>
@@ -34156,7 +34150,7 @@
     </row>
     <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>11</v>
@@ -34182,7 +34176,7 @@
     </row>
     <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>9</v>
@@ -34205,7 +34199,7 @@
     </row>
     <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>9</v>
@@ -34228,7 +34222,7 @@
     </row>
     <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>11</v>
@@ -34251,7 +34245,7 @@
     </row>
     <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>9</v>
@@ -34274,7 +34268,7 @@
     </row>
     <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B32" t="s">
         <v>9</v>
@@ -34297,7 +34291,7 @@
     </row>
     <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
@@ -34320,7 +34314,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
@@ -34343,7 +34337,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
@@ -34366,7 +34360,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
@@ -34389,7 +34383,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
@@ -34412,7 +34406,7 @@
     </row>
     <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B38" t="s">
         <v>9</v>
@@ -34435,7 +34429,7 @@
     </row>
     <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B39" t="s">
         <v>9</v>
@@ -34458,7 +34452,7 @@
     </row>
     <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
@@ -34481,7 +34475,7 @@
     </row>
     <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B41" t="s">
         <v>11</v>
@@ -34504,7 +34498,7 @@
     </row>
     <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
         <v>24</v>
@@ -34527,7 +34521,7 @@
     </row>
     <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B43" t="s">
         <v>9</v>
@@ -34550,7 +34544,7 @@
     </row>
     <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
@@ -34573,7 +34567,7 @@
     </row>
     <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B45" t="s">
         <v>16</v>
@@ -34599,7 +34593,7 @@
     </row>
     <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B46" t="s">
         <v>9</v>
@@ -34622,7 +34616,7 @@
     </row>
     <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
@@ -34645,7 +34639,7 @@
     </row>
     <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
@@ -34668,7 +34662,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
@@ -34694,7 +34688,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
@@ -34720,7 +34714,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B51" t="s">
         <v>9</v>
@@ -34743,7 +34737,7 @@
     </row>
     <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B52" t="s">
         <v>9</v>
@@ -34769,7 +34763,7 @@
     </row>
     <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B53" t="s">
         <v>9</v>
@@ -34795,7 +34789,7 @@
     </row>
     <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B54" t="s">
         <v>11</v>
@@ -34818,7 +34812,7 @@
     </row>
     <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B55" t="s">
         <v>9</v>
@@ -34841,7 +34835,7 @@
     </row>
     <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B56" t="s">
         <v>11</v>
@@ -34864,7 +34858,7 @@
     </row>
     <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
@@ -34887,7 +34881,7 @@
     </row>
     <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B58" t="s">
         <v>9</v>
@@ -34910,7 +34904,7 @@
     </row>
     <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B59" t="s">
         <v>11</v>
@@ -34933,7 +34927,7 @@
     </row>
     <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B60" t="s">
         <v>9</v>
@@ -34956,7 +34950,7 @@
     </row>
     <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B61" t="s">
         <v>9</v>
@@ -34979,7 +34973,7 @@
     </row>
     <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -35002,7 +34996,7 @@
     </row>
     <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B63" t="s">
         <v>9</v>
@@ -35028,7 +35022,7 @@
     </row>
     <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B64" t="s">
         <v>11</v>
@@ -35051,7 +35045,7 @@
     </row>
     <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B65" t="s">
         <v>9</v>
@@ -35074,7 +35068,7 @@
     </row>
     <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B66" t="s">
         <v>9</v>
@@ -35097,7 +35091,7 @@
     </row>
     <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B67" t="s">
         <v>11</v>
@@ -35123,7 +35117,7 @@
     </row>
     <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B68" t="s">
         <v>9</v>
@@ -35149,7 +35143,7 @@
     </row>
     <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B69" t="s">
         <v>9</v>
@@ -35175,7 +35169,7 @@
     </row>
     <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B70" t="s">
         <v>11</v>
@@ -35201,7 +35195,7 @@
     </row>
     <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B71" t="s">
         <v>9</v>
@@ -35227,7 +35221,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B72" t="s">
         <v>9</v>
@@ -35253,7 +35247,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B73" t="s">
         <v>11</v>
@@ -35279,7 +35273,7 @@
     </row>
     <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B74" t="s">
         <v>11</v>
@@ -35305,7 +35299,7 @@
     </row>
     <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B75" t="s">
         <v>9</v>
@@ -35331,7 +35325,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B76" t="s">
         <v>9</v>
@@ -35357,7 +35351,7 @@
     </row>
     <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B77" t="s">
         <v>9</v>
@@ -35383,7 +35377,7 @@
     </row>
     <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B78" t="s">
         <v>11</v>
@@ -35409,7 +35403,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B79" t="s">
         <v>11</v>
@@ -35435,7 +35429,7 @@
     </row>
     <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B80" t="s">
         <v>9</v>
@@ -35461,7 +35455,7 @@
     </row>
     <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B81" t="s">
         <v>11</v>
@@ -35487,7 +35481,7 @@
     </row>
     <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B82" t="s">
         <v>9</v>
@@ -35513,7 +35507,7 @@
     </row>
     <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B83" t="s">
         <v>9</v>
@@ -35539,7 +35533,7 @@
     </row>
     <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B84" t="s">
         <v>9</v>
@@ -35565,7 +35559,7 @@
     </row>
     <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B85" t="s">
         <v>9</v>
@@ -35591,7 +35585,7 @@
     </row>
     <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B86" t="s">
         <v>9</v>
@@ -35617,7 +35611,7 @@
     </row>
     <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>24</v>
@@ -35647,7 +35641,7 @@
     </row>
     <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>9</v>
@@ -35677,7 +35671,7 @@
     </row>
     <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>11</v>
@@ -35707,7 +35701,7 @@
     </row>
     <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>9</v>
@@ -35737,7 +35731,7 @@
     </row>
     <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>11</v>
@@ -35767,7 +35761,7 @@
     </row>
     <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>9</v>
@@ -35797,7 +35791,7 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>9</v>
@@ -35827,7 +35821,7 @@
     </row>
     <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>24</v>
@@ -35857,7 +35851,7 @@
     </row>
     <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>24</v>
@@ -35887,7 +35881,7 @@
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>9</v>
@@ -35917,7 +35911,7 @@
     </row>
     <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>11</v>
@@ -35947,7 +35941,7 @@
     </row>
     <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>9</v>
@@ -35977,7 +35971,7 @@
     </row>
     <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B99" t="s">
         <v>9</v>
@@ -36004,7 +35998,7 @@
     </row>
     <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B100" t="s">
         <v>24</v>
@@ -36034,7 +36028,7 @@
     </row>
     <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B101" t="s">
         <v>11</v>
@@ -36061,7 +36055,7 @@
     </row>
     <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B102" t="s">
         <v>9</v>
@@ -36089,7 +36083,7 @@
     </row>
     <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B103" t="s">
         <v>11</v>
@@ -36116,7 +36110,7 @@
     </row>
     <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B104" t="s">
         <v>11</v>
@@ -36139,7 +36133,7 @@
     </row>
     <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B105" t="s">
         <v>9</v>
@@ -36162,7 +36156,7 @@
     </row>
     <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B106" t="s">
         <v>9</v>
@@ -36185,7 +36179,7 @@
     </row>
     <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B107" t="s">
         <v>11</v>
@@ -36208,7 +36202,7 @@
     </row>
     <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B108" t="s">
         <v>9</v>
@@ -36231,7 +36225,7 @@
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B109" t="s">
         <v>11</v>
@@ -36254,7 +36248,7 @@
     </row>
     <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B110" t="s">
         <v>9</v>
@@ -36277,7 +36271,7 @@
     </row>
     <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B111" t="s">
         <v>24</v>
@@ -36300,7 +36294,7 @@
     </row>
     <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B112" t="s">
         <v>11</v>
@@ -36324,7 +36318,7 @@
     </row>
     <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B113" t="s">
         <v>11</v>
@@ -36347,7 +36341,7 @@
     </row>
     <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B114" t="s">
         <v>11</v>
@@ -36370,7 +36364,7 @@
     </row>
     <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B115" t="s">
         <v>9</v>
@@ -36393,7 +36387,7 @@
     </row>
     <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B116" t="s">
         <v>11</v>
@@ -36416,7 +36410,7 @@
     </row>
     <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B117" t="s">
         <v>9</v>
@@ -36439,7 +36433,7 @@
     </row>
     <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B118" t="s">
         <v>9</v>
@@ -36462,7 +36456,7 @@
     </row>
     <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B119" t="s">
         <v>9</v>
@@ -36485,7 +36479,7 @@
     </row>
     <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B120" t="s">
         <v>11</v>
@@ -36511,7 +36505,7 @@
     </row>
     <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B121" t="s">
         <v>9</v>
@@ -36534,7 +36528,7 @@
     </row>
     <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>9</v>
@@ -36557,7 +36551,7 @@
     </row>
     <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B123" t="s">
         <v>11</v>
@@ -36580,7 +36574,7 @@
     </row>
     <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B124" t="s">
         <v>11</v>
@@ -36656,7 +36650,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>1</v>
@@ -36771,7 +36765,7 @@
         <v>10</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>2</v>
@@ -36782,7 +36776,7 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -36819,7 +36813,7 @@
         <v>10</v>
       </c>
       <c r="Q3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -36839,7 +36833,7 @@
         <v>43636</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
@@ -36885,7 +36879,7 @@
         <v>44</v>
       </c>
       <c r="L5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P5">
         <v>21</v>
@@ -36899,7 +36893,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -36918,7 +36912,7 @@
         <v>22</v>
       </c>
       <c r="L6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -36932,7 +36926,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -36976,7 +36970,7 @@
         <v>1884</v>
       </c>
       <c r="K8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M8">
         <v>10</v>
@@ -37230,7 +37224,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -37249,7 +37243,7 @@
         <v>13</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>2</v>
@@ -37257,7 +37251,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -37288,12 +37282,12 @@
         <v>34</v>
       </c>
       <c r="O3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -37312,7 +37306,7 @@
         <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L4" t="s">
         <v>11</v>
@@ -37329,7 +37323,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -37349,7 +37343,7 @@
         <v>84</v>
       </c>
       <c r="K5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L5" t="s">
         <v>9</v>
@@ -37363,7 +37357,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -37382,7 +37376,7 @@
         <v>7</v>
       </c>
       <c r="K6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L6" t="s">
         <v>11</v>
@@ -37396,7 +37390,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -37426,7 +37420,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -37445,7 +37439,7 @@
         <v>7</v>
       </c>
       <c r="K8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L8" t="s">
         <v>11</v>
@@ -37459,7 +37453,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -37489,7 +37483,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -37508,7 +37502,7 @@
         <v>7</v>
       </c>
       <c r="K10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L10" t="s">
         <v>11</v>
@@ -37522,7 +37516,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -37552,7 +37546,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -37571,7 +37565,7 @@
         <v>14</v>
       </c>
       <c r="K12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M12">
         <v>225</v>
@@ -37585,7 +37579,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -37609,7 +37603,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -37632,7 +37626,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>9</v>
@@ -37655,7 +37649,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
@@ -37678,7 +37672,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
@@ -37795,7 +37789,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -37814,7 +37808,7 @@
         <v>57</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>2</v>
@@ -37822,7 +37816,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
@@ -37853,12 +37847,12 @@
         <v>34</v>
       </c>
       <c r="O3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -37877,7 +37871,7 @@
         <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L4" t="s">
         <v>9</v>
@@ -37891,7 +37885,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -37922,7 +37916,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -37941,7 +37935,7 @@
         <v>58</v>
       </c>
       <c r="K6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M6">
         <v>129</v>
@@ -37952,7 +37946,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -37971,7 +37965,7 @@
         <v>72</v>
       </c>
       <c r="K7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L7" t="s">
         <v>24</v>
@@ -37985,7 +37979,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -38004,7 +37998,7 @@
         <v>7</v>
       </c>
       <c r="K8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N8">
         <v>34</v>
@@ -38015,7 +38009,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -38034,7 +38028,7 @@
         <v>10</v>
       </c>
       <c r="K9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L9" t="s">
         <v>9</v>
@@ -38048,7 +38042,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -38078,7 +38072,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -38097,7 +38091,7 @@
         <v>3</v>
       </c>
       <c r="K11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M11">
         <v>100</v>
@@ -38115,7 +38109,7 @@
         <v>45569</v>
       </c>
       <c r="K12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L12" t="s">
         <v>9</v>
@@ -38136,7 +38130,7 @@
         <v>45569</v>
       </c>
       <c r="K13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M13">
         <v>10</v>
@@ -38156,7 +38150,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M14">
         <v>239</v>
@@ -38298,7 +38292,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -38320,7 +38314,7 @@
         <v>5</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>2</v>
@@ -38328,7 +38322,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -38359,12 +38353,12 @@
         <v>10</v>
       </c>
       <c r="O3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -38383,7 +38377,7 @@
         <v>22</v>
       </c>
       <c r="K4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L4" t="s">
         <v>24</v>
@@ -38397,7 +38391,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -38417,7 +38411,7 @@
         <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M5">
         <v>5</v>
@@ -38428,7 +38422,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -38447,7 +38441,7 @@
         <v>14</v>
       </c>
       <c r="K6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L6" t="s">
         <v>9</v>
@@ -38461,7 +38455,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -38491,7 +38485,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -38510,7 +38504,7 @@
         <v>3</v>
       </c>
       <c r="K8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N8">
         <v>114</v>
@@ -38521,7 +38515,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
         <v>24</v>
@@ -38540,7 +38534,7 @@
         <v>5</v>
       </c>
       <c r="K9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L9" t="s">
         <v>9</v>
@@ -38554,7 +38548,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
         <v>24</v>
@@ -38573,7 +38567,7 @@
         <v>5</v>
       </c>
       <c r="K10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N10">
         <v>5</v>
@@ -38584,7 +38578,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -38603,7 +38597,7 @@
         <v>2</v>
       </c>
       <c r="K11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L11" t="s">
         <v>24</v>
@@ -38617,7 +38611,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -38647,7 +38641,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -38666,7 +38660,7 @@
         <v>16</v>
       </c>
       <c r="K13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M13">
         <v>5</v>
@@ -38689,7 +38683,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L14" t="s">
         <v>24</v>
@@ -38712,7 +38706,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M15">
         <v>5</v>
@@ -38732,7 +38726,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M16">
         <v>15</v>
@@ -38852,7 +38846,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -38874,7 +38868,7 @@
         <v>5</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>2</v>
@@ -38882,7 +38876,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -38919,12 +38913,12 @@
         <v>34</v>
       </c>
       <c r="P3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -38946,7 +38940,7 @@
         <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L4" t="s">
         <v>9</v>
@@ -38960,7 +38954,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -38982,7 +38976,7 @@
         <v>8</v>
       </c>
       <c r="K5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M5">
         <v>21</v>
@@ -38993,7 +38987,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -39012,7 +39006,7 @@
         <v>7</v>
       </c>
       <c r="K6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L6" t="s">
         <v>11</v>
@@ -39026,7 +39020,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -39045,7 +39039,7 @@
         <v>5</v>
       </c>
       <c r="K7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L7" t="s">
         <v>9</v>
@@ -39059,7 +39053,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -39081,7 +39075,7 @@
         <v>8</v>
       </c>
       <c r="K8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M8">
         <v>96</v>
@@ -39092,7 +39086,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -39111,7 +39105,7 @@
         <v>7</v>
       </c>
       <c r="K9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L9" t="s">
         <v>11</v>
@@ -39128,7 +39122,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -39147,7 +39141,7 @@
         <v>13</v>
       </c>
       <c r="K10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L10" t="s">
         <v>9</v>
@@ -39164,7 +39158,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -39183,7 +39177,7 @@
         <v>7</v>
       </c>
       <c r="K11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M11">
         <v>56</v>
@@ -39200,7 +39194,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -39219,7 +39213,7 @@
         <v>8</v>
       </c>
       <c r="K12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L12" t="s">
         <v>11</v>
@@ -39233,7 +39227,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -39252,7 +39246,7 @@
         <v>30</v>
       </c>
       <c r="K13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L13" t="s">
         <v>9</v>
@@ -39266,7 +39260,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -39287,7 +39281,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M14">
         <v>49</v>
@@ -39298,7 +39292,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
@@ -39319,7 +39313,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L15" t="s">
         <v>9</v>
@@ -39333,7 +39327,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
@@ -39354,7 +39348,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M16">
         <v>26</v>
@@ -39365,7 +39359,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
@@ -39386,7 +39380,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
@@ -39407,7 +39401,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
@@ -39428,7 +39422,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
@@ -39452,7 +39446,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
@@ -39536,7 +39530,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -39555,7 +39549,7 @@
         <v>40</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>2</v>
@@ -39563,7 +39557,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -39594,12 +39588,12 @@
         <v>13</v>
       </c>
       <c r="P3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -39621,7 +39615,7 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M4" t="s">
         <v>11</v>
@@ -39635,7 +39629,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -39657,7 +39651,7 @@
         <v>14</v>
       </c>
       <c r="L5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M5" t="s">
         <v>9</v>
@@ -39671,7 +39665,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -39690,7 +39684,7 @@
         <v>7</v>
       </c>
       <c r="L6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N6">
         <v>68</v>
@@ -39701,7 +39695,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -39723,7 +39717,7 @@
         <v>3</v>
       </c>
       <c r="L7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M7" t="s">
         <v>11</v>
@@ -39737,7 +39731,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -39759,7 +39753,7 @@
         <v>3</v>
       </c>
       <c r="L8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M8" t="s">
         <v>9</v>
@@ -39773,7 +39767,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -39792,7 +39786,7 @@
         <v>4</v>
       </c>
       <c r="L9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N9">
         <v>22</v>
@@ -39803,7 +39797,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -39822,7 +39816,7 @@
         <v>14</v>
       </c>
       <c r="L10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M10" t="s">
         <v>9</v>
@@ -39836,7 +39830,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -39855,7 +39849,7 @@
         <v>7</v>
       </c>
       <c r="L11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="O11">
         <v>3</v>
@@ -39866,7 +39860,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -39885,7 +39879,7 @@
         <v>7</v>
       </c>
       <c r="L12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M12" t="s">
         <v>11</v>
@@ -39902,7 +39896,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -39921,7 +39915,7 @@
         <v>6</v>
       </c>
       <c r="L13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M13" t="s">
         <v>9</v>
@@ -39938,7 +39932,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -39960,7 +39954,7 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N14">
         <v>68</v>
@@ -39974,7 +39968,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
@@ -39996,7 +39990,7 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M15" t="s">
         <v>11</v>
@@ -40010,7 +40004,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -40032,7 +40026,7 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M16" t="s">
         <v>9</v>
@@ -40046,7 +40040,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
@@ -40065,7 +40059,7 @@
         <v>7</v>
       </c>
       <c r="L17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N17">
         <v>91</v>
@@ -40076,7 +40070,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
@@ -40100,7 +40094,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
@@ -40121,7 +40115,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
@@ -40142,7 +40136,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
@@ -40226,7 +40220,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -40245,7 +40239,7 @@
         <v>43</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>2</v>
@@ -40253,7 +40247,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -40284,12 +40278,12 @@
         <v>13</v>
       </c>
       <c r="O3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -40308,7 +40302,7 @@
         <v>6</v>
       </c>
       <c r="K4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L4" t="s">
         <v>9</v>
@@ -40322,7 +40316,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -40341,7 +40335,7 @@
         <v>15</v>
       </c>
       <c r="K5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M5">
         <v>43</v>
@@ -40352,7 +40346,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -40371,7 +40365,7 @@
         <v>19</v>
       </c>
       <c r="K6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L6" t="s">
         <v>11</v>
@@ -40385,7 +40379,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -40404,7 +40398,7 @@
         <v>5</v>
       </c>
       <c r="K7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N7">
         <v>10</v>
@@ -40415,7 +40409,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -40434,7 +40428,7 @@
         <v>37</v>
       </c>
       <c r="K8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L8" t="s">
         <v>9</v>
@@ -40448,7 +40442,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -40467,7 +40461,7 @@
         <v>43</v>
       </c>
       <c r="K9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L9" t="s">
         <v>11</v>
@@ -40481,7 +40475,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -40500,7 +40494,7 @@
         <v>3</v>
       </c>
       <c r="K10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M10">
         <v>45</v>
@@ -40511,7 +40505,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -40530,7 +40524,7 @@
         <v>2</v>
       </c>
       <c r="K11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L11" t="s">
         <v>9</v>
@@ -40544,7 +40538,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
@@ -40563,7 +40557,7 @@
         <v>3</v>
       </c>
       <c r="K12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M12">
         <v>37</v>
@@ -40574,7 +40568,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -40593,7 +40587,7 @@
         <v>7</v>
       </c>
       <c r="K13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L13" t="s">
         <v>9</v>
@@ -40607,7 +40601,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -40628,7 +40622,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M14">
         <v>43</v>
@@ -40639,7 +40633,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -40663,7 +40657,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L15" t="s">
         <v>9</v>
@@ -40677,7 +40671,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -40698,7 +40692,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L16" t="s">
         <v>11</v>
@@ -40717,7 +40711,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="K17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N17">
         <v>5</v>
@@ -40733,7 +40727,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="K18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L18" t="s">
         <v>24</v>
@@ -40752,7 +40746,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="K19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N19">
         <v>3</v>
@@ -40768,7 +40762,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="K20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L20" t="s">
         <v>9</v>
@@ -40787,7 +40781,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="K21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L21" t="s">
         <v>16</v>
@@ -40806,7 +40800,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="K22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M22">
         <v>63</v>
@@ -40888,15 +40882,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A894341C42F9B24A906E167E11DF703F" ma:contentTypeVersion="17" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="3d82bd73d8a4c338bf424a08b3fb8c4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0f9b4a4b-bf3c-4b0e-80e3-81e6d49e70bb" xmlns:ns3="cb68a5bd-8a64-4a69-8df9-ff13e1702013" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c1bac0ed0a8d32072afc7c59cebfc1a" ns2:_="" ns3:_="">
     <xsd:import namespace="0f9b4a4b-bf3c-4b0e-80e3-81e6d49e70bb"/>
@@ -41145,15 +41130,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E8797C-0731-4E57-9BFF-CC6377F8CCD8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{992E78AC-BA2F-49A2-81B4-F312A9AD36D8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41170,4 +41156,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E8797C-0731-4E57-9BFF-CC6377F8CCD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>